<commit_message>
Added GEUS 2022 notes + small update on existing files
</commit_message>
<xml_diff>
--- a/Field books/digitized by BAV from JEBs green folder.xlsx
+++ b/Field books/digitized by BAV from JEBs green folder.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bav\OneDrive - Geological survey of Denmark and Greenland\Code\PROMICE\GC-Net-Level-1-data-processing\metadata\Field Books\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bav\OneDrive - Geological survey of Denmark and Greenland\Code\PROMICE\GC-Net-historical-metadata\Field books\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_308489C7AD5DB79DAC25CB8169B5A9D381F39C71" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6C39140A-D781-4CA5-B436-E8CDEFC8FA56}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_308489C7AD5DB79DAC25CB8169B5A9D381F39C71" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5FAD6C82-214D-4ABE-A96E-8FD420452BC7}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="2160" windowWidth="23040" windowHeight="6180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -207,12 +207,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -227,9 +233,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -581,175 +589,184 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
+      <c r="A1" s="2">
         <v>35945</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>17</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>47</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>65</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>46</v>
       </c>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>172</v>
       </c>
+      <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3">
         <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3">
         <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3">
         <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+      <c r="A11" s="2">
         <v>35945</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>51</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>25</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>85</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="3">
         <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>51</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="3">
         <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="3">
         <v>51</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="3">
         <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="3">
         <v>120</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="3">
         <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="3">
         <v>205</v>
       </c>
+      <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="3">
         <v>205</v>
       </c>
+      <c r="C19" s="3"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">

</xml_diff>